<commit_message>
Updated schematic, PSU added + draft program
</commit_message>
<xml_diff>
--- a/BOM/BOM UPZ Switcher.xlsx
+++ b/BOM/BOM UPZ Switcher.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bart\Documents\GitHub\UPZ_Switcher\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4DE537-1206-4601-84C6-44C55F7F5538}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F88592-42CD-44F6-9B0A-C4F97A72F6D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4830" yWindow="4755" windowWidth="21600" windowHeight="11505" xr2:uid="{3C56C210-DCD0-4B76-B854-73BBFDBB2958}"/>
+    <workbookView xWindow="4830" yWindow="4245" windowWidth="21600" windowHeight="11505" xr2:uid="{3C56C210-DCD0-4B76-B854-73BBFDBB2958}"/>
   </bookViews>
   <sheets>
     <sheet name="FetHead" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
   <si>
     <t>Description</t>
   </si>
@@ -157,6 +157,12 @@
   </si>
   <si>
     <t>1N4148</t>
+  </si>
+  <si>
+    <t>DIP Switch</t>
+  </si>
+  <si>
+    <t>Address selector</t>
   </si>
 </sst>
 </file>
@@ -525,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B339EA2E-58E6-48C2-B743-24C662D28A88}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,11 +863,22 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E22" t="s">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
         <v>10</v>
       </c>
-      <c r="F22">
+      <c r="F23">
         <f>SUM(F2:F15)</f>
         <v>108.93600000000001</v>
       </c>

</xml_diff>

<commit_message>
update on power supply
</commit_message>
<xml_diff>
--- a/BOM/BOM UPZ Switcher.xlsx
+++ b/BOM/BOM UPZ Switcher.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bart\Documents\GitHub\UPZ_Switcher\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED68C337-8068-48A5-976E-2DAE630FFE94}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F525503-4ABF-47FE-948E-620F9FDAF69B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4830" yWindow="4245" windowWidth="21600" windowHeight="11505" xr2:uid="{3C56C210-DCD0-4B76-B854-73BBFDBB2958}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
   <si>
     <t>Description</t>
   </si>
@@ -169,6 +169,27 @@
   </si>
   <si>
     <t>Receptacle 10</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>1-726386-2</t>
+  </si>
+  <si>
+    <t>Screws</t>
+  </si>
+  <si>
+    <t>Mouser</t>
+  </si>
+  <si>
+    <t>IEC Filter</t>
+  </si>
+  <si>
+    <t>ACDC 48V</t>
+  </si>
+  <si>
+    <t>ACDC 5V</t>
   </si>
 </sst>
 </file>
@@ -537,14 +558,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B339EA2E-58E6-48C2-B743-24C662D28A88}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.140625" customWidth="1"/>
@@ -902,11 +924,63 @@
         <v>2</v>
       </c>
     </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E26" t="s">
+      <c r="A26" s="1">
+        <v>2992519</v>
+      </c>
+      <c r="B26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>2671563</v>
+      </c>
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>3583986</v>
+      </c>
+      <c r="B28" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
         <v>10</v>
       </c>
-      <c r="F26">
+      <c r="F30">
         <f>SUM(F2:F15)</f>
         <v>108.93600000000001</v>
       </c>
@@ -922,8 +996,12 @@
     <hyperlink ref="A8" r:id="rId6" xr:uid="{7C032C1A-3DAB-485E-B8EB-E9C947593005}"/>
     <hyperlink ref="A23" r:id="rId7" display="1103937" xr:uid="{7A8246D9-2FF3-4722-A34A-AD1A61A9833B}"/>
     <hyperlink ref="A22" r:id="rId8" display="1103961" xr:uid="{033BBA22-0713-46D5-8340-4FC998548605}"/>
+    <hyperlink ref="A24" r:id="rId9" xr:uid="{D79EAC5C-97E9-4F55-854B-1E260CFD452E}"/>
+    <hyperlink ref="A26" r:id="rId10" display="2992519" xr:uid="{C9C3755A-9D99-4B8E-8E03-6E7357E2AD15}"/>
+    <hyperlink ref="A27" r:id="rId11" display="2671563" xr:uid="{B377D999-965E-424A-8DED-683DA1A584E8}"/>
+    <hyperlink ref="A28" r:id="rId12" display="3583986" xr:uid="{45099F28-E9F6-4702-8FA0-3949CA6A5D10}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>